<commit_message>
Poster acabado. Mockups, relatorio e Gantt atualizados
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt.xlsx
+++ b/Diagrama de Gantt.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85624737-E16D-4A3D-B767-CEFF63EE53C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{17E7C974-1295-454C-BF79-D11EE1356D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3060" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="16" r:id="rId1"/>
@@ -13,8 +13,8 @@
   <definedNames>
     <definedName name="Hoje" localSheetId="0">TODAY()</definedName>
     <definedName name="Incremento_de_Deslocamento" localSheetId="0">Gantt!$C$7</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Gantt!$6:$9</definedName>
     <definedName name="Projeto_Início" localSheetId="0">Gantt!$C$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Gantt!$6:$9</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -173,11 +173,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="d"/>
-    <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="d"/>
+    <numFmt numFmtId="165" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,7 +561,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -573,7 +573,7 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -598,16 +598,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -623,7 +623,7 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -658,13 +658,13 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -709,7 +709,7 @@
     <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -719,7 +719,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -769,48 +769,34 @@
     </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Cabeçalho 1" xfId="6" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 2" xfId="7" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Comma [0]" xfId="10" builtinId="6" customBuiltin="1"/>
     <cellStyle name="Data" xfId="9" xr:uid="{229918B6-DD13-4F5A-97B9-305F7E002AA3}"/>
-    <cellStyle name="Hiperligação" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentagem" xfId="2" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Separador de milhares [0]" xfId="10" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Vírgula" xfId="4" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zTextoOculto" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="31">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color theme="0"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+        <patternFill>
+          <bgColor theme="1" tint="0.34998626667073579"/>
         </patternFill>
       </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -872,22 +858,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
         </patternFill>
       </fill>
       <border>
@@ -1016,6 +986,36 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1354,8 +1354,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Marcos435" displayName="Marcos435" ref="B9:G25" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Marcos435" displayName="Marcos435" ref="B9:G25" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="B9:G25" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1365,9 +1369,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6E47A83D-ACD7-4EB6-9B84-5195E813945E}" name="Descrição do marco" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{529EEF64-D037-4ACF-8CA4-0C10FE2D1FBB}" name="Categoria" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{711D01BA-2785-403A-9636-CCC7E2ADA584}" name="Atribuído a" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6E47A83D-ACD7-4EB6-9B84-5195E813945E}" name="Descrição do marco" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{529EEF64-D037-4ACF-8CA4-0C10FE2D1FBB}" name="Categoria" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{711D01BA-2785-403A-9636-CCC7E2ADA584}" name="Atribuído a" dataDxfId="14"/>
     <tableColumn id="4" xr3:uid="{62B00BEF-16BE-4692-B5E2-F287F680F2C1}" name="Progresso"/>
     <tableColumn id="5" xr3:uid="{D6D72902-F68F-4E59-A714-AFFF520C647A}" name="Início" dataCellStyle="Data"/>
     <tableColumn id="6" xr3:uid="{93E698DE-286F-49ED-AA20-D0C843671DE8}" name="Dias"/>
@@ -1696,11 +1700,11 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:BP25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A9" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
@@ -1713,8 +1717,8 @@
     <col min="9" max="65" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="25.15" customHeight="1"/>
-    <row r="2" spans="1:68" ht="49.9" customHeight="1">
+    <row r="1" spans="1:68" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1785,7 +1789,7 @@
       <c r="BL2" s="13"/>
       <c r="BM2" s="13"/>
     </row>
-    <row r="3" spans="1:68" ht="19.899999999999999" customHeight="1">
+    <row r="3" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="34"/>
       <c r="C3" s="35"/>
@@ -1852,7 +1856,7 @@
       <c r="BL3" s="24"/>
       <c r="BM3" s="24"/>
     </row>
-    <row r="4" spans="1:68" ht="30" customHeight="1">
+    <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="45" t="s">
         <v>2</v>
@@ -1929,7 +1933,7 @@
       <c r="BL4" s="24"/>
       <c r="BM4" s="24"/>
     </row>
-    <row r="5" spans="1:68" ht="30" customHeight="1">
+    <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -2008,7 +2012,7 @@
       <c r="BL5" s="24"/>
       <c r="BM5" s="24"/>
     </row>
-    <row r="6" spans="1:68" ht="30" customHeight="1">
+    <row r="6" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="41" t="s">
         <v>13</v>
@@ -2023,7 +2027,7 @@
       <c r="H6" s="21"/>
       <c r="I6" s="49" t="str">
         <f ca="1">TEXT(I7,"mmmm")</f>
-        <v>outubro</v>
+        <v>October</v>
       </c>
       <c r="J6" s="49"/>
       <c r="K6" s="49"/>
@@ -2073,7 +2077,7 @@
       <c r="AQ6" s="49"/>
       <c r="AR6" s="49" t="str">
         <f ca="1">IF(OR(TEXT(AR7,"mmmm")=AK6,TEXT(AR7,"mmmm")=AD6,TEXT(AR7,"mmmm")=W6,TEXT(AR7,"mmmm")=P6),"",TEXT(AR7,"mmmm"))</f>
-        <v>novembro</v>
+        <v>November</v>
       </c>
       <c r="AS6" s="49"/>
       <c r="AT6" s="49"/>
@@ -2103,7 +2107,7 @@
       <c r="BL6" s="48"/>
       <c r="BM6" s="24"/>
     </row>
-    <row r="7" spans="1:68" ht="30" customHeight="1">
+    <row r="7" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="41" t="s">
         <v>14</v>
@@ -2342,7 +2346,7 @@
       </c>
       <c r="BM7" s="24"/>
     </row>
-    <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1">
+    <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="43"/>
       <c r="C8" s="43"/>
@@ -2409,7 +2413,7 @@
       <c r="BL8" s="31"/>
       <c r="BM8" s="24"/>
     </row>
-    <row r="9" spans="1:68" ht="40.15" customHeight="1">
+    <row r="9" spans="1:68" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -2434,231 +2438,231 @@
       <c r="H9" s="40"/>
       <c r="I9" s="29" t="str">
         <f t="shared" ref="I9:BL9" ca="1" si="3">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>t</v>
+        <v>T</v>
       </c>
       <c r="J9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>W</v>
       </c>
       <c r="K9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>T</v>
       </c>
       <c r="L9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>F</v>
       </c>
       <c r="M9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="N9" s="29" t="str">
         <f ca="1">LEFT(TEXT(N7,"ddd"),1)</f>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="O9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>M</v>
       </c>
       <c r="P9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>T</v>
       </c>
       <c r="Q9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>W</v>
       </c>
       <c r="R9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>T</v>
       </c>
       <c r="S9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>F</v>
       </c>
       <c r="T9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="U9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="V9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>M</v>
       </c>
       <c r="W9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>T</v>
       </c>
       <c r="X9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>W</v>
       </c>
       <c r="Y9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>T</v>
       </c>
       <c r="Z9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>F</v>
       </c>
       <c r="AA9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="AB9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="AC9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>M</v>
       </c>
       <c r="AD9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>T</v>
       </c>
       <c r="AE9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>W</v>
       </c>
       <c r="AF9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>T</v>
       </c>
       <c r="AG9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>F</v>
       </c>
       <c r="AH9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="AI9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="AJ9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>M</v>
       </c>
       <c r="AK9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>T</v>
       </c>
       <c r="AL9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>W</v>
       </c>
       <c r="AM9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>T</v>
       </c>
       <c r="AN9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>F</v>
       </c>
       <c r="AO9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="AP9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="AQ9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>M</v>
       </c>
       <c r="AR9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>T</v>
       </c>
       <c r="AS9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>W</v>
       </c>
       <c r="AT9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>T</v>
       </c>
       <c r="AU9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>F</v>
       </c>
       <c r="AV9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="AW9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="AX9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>M</v>
       </c>
       <c r="AY9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>T</v>
       </c>
       <c r="AZ9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>W</v>
       </c>
       <c r="BA9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>T</v>
       </c>
       <c r="BB9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>F</v>
       </c>
       <c r="BC9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="BD9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="BE9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>M</v>
       </c>
       <c r="BF9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>t</v>
+        <v>T</v>
       </c>
       <c r="BG9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>W</v>
       </c>
       <c r="BH9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>q</v>
+        <v>T</v>
       </c>
       <c r="BI9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>F</v>
       </c>
       <c r="BJ9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="BK9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="BL9" s="29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>M</v>
       </c>
       <c r="BM9" s="24"/>
     </row>
-    <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" thickBot="1">
+    <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
       <c r="C10" s="6"/>
       <c r="D10" s="5"/>
@@ -2724,7 +2728,7 @@
       <c r="BL10" s="28"/>
       <c r="BM10" s="24"/>
     </row>
-    <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1">
+    <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -2967,7 +2971,7 @@
       <c r="BM11" s="20"/>
       <c r="BP11" s="33"/>
     </row>
-    <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1">
+    <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="18" t="s">
         <v>25</v>
@@ -2979,7 +2983,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="15">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F12" s="16">
         <v>45580</v>
@@ -3214,7 +3218,7 @@
       </c>
       <c r="BM12" s="20"/>
     </row>
-    <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1">
+    <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="18" t="s">
         <v>27</v>
@@ -3461,7 +3465,7 @@
       </c>
       <c r="BM13" s="20"/>
     </row>
-    <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1">
+    <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="18" t="s">
         <v>28</v>
@@ -3479,7 +3483,7 @@
         <v>45584</v>
       </c>
       <c r="G14" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="39" t="str">
@@ -3708,7 +3712,7 @@
       </c>
       <c r="BM14" s="20"/>
     </row>
-    <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1">
+    <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="56" t="s">
         <v>30</v>
@@ -3787,7 +3791,7 @@
       <c r="BL15" s="19"/>
       <c r="BM15" s="20"/>
     </row>
-    <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1">
+    <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="54" t="s">
         <v>31</v>
@@ -4030,7 +4034,7 @@
       </c>
       <c r="BM16" s="20"/>
     </row>
-    <row r="17" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1">
+    <row r="17" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="18" t="s">
         <v>32</v>
@@ -4277,7 +4281,7 @@
       </c>
       <c r="BM17" s="20"/>
     </row>
-    <row r="18" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1">
+    <row r="18" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="18" t="s">
         <v>33</v>
@@ -4524,7 +4528,7 @@
       </c>
       <c r="BM18" s="20"/>
     </row>
-    <row r="19" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1">
+    <row r="19" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="18" t="s">
         <v>34</v>
@@ -4771,7 +4775,7 @@
       </c>
       <c r="BM19" s="20"/>
     </row>
-    <row r="20" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1">
+    <row r="20" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="18" t="s">
         <v>35</v>
@@ -5018,7 +5022,7 @@
       </c>
       <c r="BM20" s="20"/>
     </row>
-    <row r="21" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1">
+    <row r="21" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="54" t="s">
         <v>36</v>
@@ -5261,7 +5265,7 @@
       </c>
       <c r="BM21" s="20"/>
     </row>
-    <row r="22" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1">
+    <row r="22" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="18" t="s">
         <v>37</v>
@@ -5508,7 +5512,7 @@
       </c>
       <c r="BM22" s="20"/>
     </row>
-    <row r="23" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1">
+    <row r="23" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="18" t="s">
         <v>38</v>
@@ -5755,7 +5759,7 @@
       </c>
       <c r="BM23" s="20"/>
     </row>
-    <row r="24" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1">
+    <row r="24" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="18" t="s">
         <v>39</v>
@@ -6002,7 +6006,7 @@
       </c>
       <c r="BM24" s="20"/>
     </row>
-    <row r="25" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1">
+    <row r="25" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="18" t="s">
         <v>40</v>
@@ -6275,57 +6279,57 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="17" priority="10">
+    <cfRule type="expression" dxfId="13" priority="10">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="16" priority="8">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL25">
-    <cfRule type="expression" dxfId="15" priority="7">
+    <cfRule type="expression" dxfId="11" priority="7">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL21">
-    <cfRule type="expression" dxfId="14" priority="194" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="194" stopIfTrue="1">
       <formula>AND($C10="Risco Baixo",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="195" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="195" stopIfTrue="1">
       <formula>AND($C10="Risco Elevado",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="196" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="196" stopIfTrue="1">
       <formula>AND($C10="Dentro do prazo",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="197" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="197" stopIfTrue="1">
       <formula>AND($C10="Risco Médio",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="198" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="198" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="9" priority="9">
-      <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
+  <conditionalFormatting sqref="I22:BL25">
+    <cfRule type="expression" dxfId="5" priority="212" stopIfTrue="1">
+      <formula>AND($C22="Risco Baixo",I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="213" stopIfTrue="1">
+      <formula>AND($C22="Risco Elevado",I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="214" stopIfTrue="1">
+      <formula>AND($C22="Dentro do prazo",I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="215" stopIfTrue="1">
+      <formula>AND($C22="Risco Médio",I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="216" stopIfTrue="1">
+      <formula>AND(LEN($C22)=0,I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22:BL25">
-    <cfRule type="expression" dxfId="8" priority="212" stopIfTrue="1">
-      <formula>AND($C22="Risco Baixo",I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="213" stopIfTrue="1">
-      <formula>AND($C22="Risco Elevado",I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="214" stopIfTrue="1">
-      <formula>AND($C22="Dentro do prazo",I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="215" stopIfTrue="1">
-      <formula>AND($C22="Risco Médio",I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="216" stopIfTrue="1">
-      <formula>AND(LEN($C22)=0,I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
+  <conditionalFormatting sqref="J6:BL6">
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="10">
@@ -6722,15 +6726,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -6749,14 +6744,59 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C87518-DD8E-42CD-8DAC-291A323E849B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C87518-DD8E-42CD-8DAC-291A323E849B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Poster finalizado com QR code e Gantt atualizado
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt.xlsx
+++ b/Diagrama de Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17E7C974-1295-454C-BF79-D11EE1356D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F9B9BD-4AC4-4758-891E-8F5885485CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3060" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1354,10 +1354,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Marcos435" displayName="Marcos435" ref="B9:G25" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="B9:G25" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
@@ -1700,8 +1696,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:BP25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2989,7 +2985,7 @@
         <v>45580</v>
       </c>
       <c r="G12" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="39" t="str">
@@ -3236,7 +3232,7 @@
         <v>45579</v>
       </c>
       <c r="G13" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="39" t="str">
@@ -3483,7 +3479,7 @@
         <v>45584</v>
       </c>
       <c r="G14" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="39" t="str">
@@ -4293,7 +4289,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="15">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F18" s="16">
         <v>45589</v>
@@ -6450,6 +6446,34 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="22a266b9fa9a230c5a512669d8b298c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eddc33fff6b14141ee5c74a0d29ea6a1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6725,51 +6749,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C87518-DD8E-42CD-8DAC-291A323E849B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6794,9 +6777,22 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C87518-DD8E-42CD-8DAC-291A323E849B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Logótipo adicionado, Poster e Gantt atualizados
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt.xlsx
+++ b/Diagrama de Gantt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F9B9BD-4AC4-4758-891E-8F5885485CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758E54E8-69E9-4875-B4B2-C8B260D52C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="16" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Criar um diagrama de Gantt 
 Introduzir o título deste projeto na célula B2. 
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Versão final da app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Logótipo</t>
+  </si>
+  <si>
+    <t>Risco Baixo</t>
   </si>
 </sst>
 </file>
@@ -1355,8 +1361,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Marcos435" displayName="Marcos435" ref="B9:G25" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="B9:G25" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Marcos435" displayName="Marcos435" ref="B9:G26" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="B9:G26" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1694,10 +1700,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537EAE25-AFCC-4679-A578-F5918B332482}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:BP25"/>
+  <dimension ref="A1:BP26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2744,7 +2750,7 @@
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="39" t="str">
-        <f t="shared" ref="I11:X25" ca="1" si="4">IF(AND($C11="Objetivo",I$7&gt;=$F11,I$7&lt;=$F11+$G11-1),2,IF(AND($C11="Marco",I$7&gt;=$F11,I$7&lt;=$F11+$G11-1),1,""))</f>
+        <f t="shared" ref="I11:X26" ca="1" si="4">IF(AND($C11="Objetivo",I$7&gt;=$F11,I$7&lt;=$F11+$G11-1),2,IF(AND($C11="Marco",I$7&gt;=$F11,I$7&lt;=$F11+$G11-1),1,""))</f>
         <v/>
       </c>
       <c r="J11" s="19"/>
@@ -2805,7 +2811,7 @@
         <v/>
       </c>
       <c r="Y11" s="19" t="str">
-        <f t="shared" ref="Y11:AN25" ca="1" si="5">IF(AND($C11="Objetivo",Y$7&gt;=$F11,Y$7&lt;=$F11+$G11-1),2,IF(AND($C11="Marco",Y$7&gt;=$F11,Y$7&lt;=$F11+$G11-1),1,""))</f>
+        <f t="shared" ref="Y11:AN26" ca="1" si="5">IF(AND($C11="Objetivo",Y$7&gt;=$F11,Y$7&lt;=$F11+$G11-1),2,IF(AND($C11="Marco",Y$7&gt;=$F11,Y$7&lt;=$F11+$G11-1),1,""))</f>
         <v/>
       </c>
       <c r="Z11" s="19" t="str">
@@ -2869,7 +2875,7 @@
         <v/>
       </c>
       <c r="AO11" s="19" t="str">
-        <f t="shared" ref="AO11:BD25" ca="1" si="6">IF(AND($C11="Objetivo",AO$7&gt;=$F11,AO$7&lt;=$F11+$G11-1),2,IF(AND($C11="Marco",AO$7&gt;=$F11,AO$7&lt;=$F11+$G11-1),1,""))</f>
+        <f t="shared" ref="AO11:BD26" ca="1" si="6">IF(AND($C11="Objetivo",AO$7&gt;=$F11,AO$7&lt;=$F11+$G11-1),2,IF(AND($C11="Marco",AO$7&gt;=$F11,AO$7&lt;=$F11+$G11-1),1,""))</f>
         <v/>
       </c>
       <c r="AP11" s="19" t="str">
@@ -2933,7 +2939,7 @@
         <v/>
       </c>
       <c r="BE11" s="19" t="str">
-        <f t="shared" ref="BE11:BL25" ca="1" si="7">IF(AND($C11="Objetivo",BE$7&gt;=$F11,BE$7&lt;=$F11+$G11-1),2,IF(AND($C11="Marco",BE$7&gt;=$F11,BE$7&lt;=$F11+$G11-1),1,""))</f>
+        <f t="shared" ref="BE11:BL26" ca="1" si="7">IF(AND($C11="Objetivo",BE$7&gt;=$F11,BE$7&lt;=$F11+$G11-1),2,IF(AND($C11="Marco",BE$7&gt;=$F11,BE$7&lt;=$F11+$G11-1),1,""))</f>
         <v/>
       </c>
       <c r="BF11" s="19" t="str">
@@ -3236,7 +3242,7 @@
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="39" t="str">
-        <f t="shared" ref="I13:I25" ca="1" si="8">IF(AND($C13="Objetivo",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),2,IF(AND($C13="Marco",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),1,""))</f>
+        <f t="shared" ref="I13:I26" ca="1" si="8">IF(AND($C13="Objetivo",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),2,IF(AND($C13="Marco",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),1,""))</f>
         <v/>
       </c>
       <c r="J13" s="19" t="str">
@@ -3788,267 +3794,99 @@
       <c r="BM15" s="20"/>
     </row>
     <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="54" t="s">
-        <v>31</v>
+      <c r="A16" s="3"/>
+      <c r="B16" s="56" t="s">
+        <v>41</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
+        <v>42</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="15">
+        <v>1</v>
+      </c>
       <c r="F16" s="16">
-        <v>45620</v>
+        <v>45584</v>
       </c>
       <c r="G16" s="17">
         <v>1</v>
       </c>
       <c r="H16" s="12"/>
-      <c r="I16" s="39" t="str">
-        <f t="shared" ca="1" si="8"/>
-        <v/>
-      </c>
-      <c r="J16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="K16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="L16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="M16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="N16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="O16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="P16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="Q16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="R16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="S16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="T16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="U16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="V16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="W16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="X16" s="19" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="Y16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="Z16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AA16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AB16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AC16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AD16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AE16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AF16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AG16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AH16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AI16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AJ16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AK16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AL16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AM16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AN16" s="19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="AO16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AP16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AQ16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AR16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AS16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AT16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AU16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AV16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AW16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AX16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AY16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AZ16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BA16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BB16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BC16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BD16" s="19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="BE16" s="19" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BF16" s="19" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BG16" s="19" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BH16" s="19" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BI16" s="19" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BJ16" s="19" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="BK16" s="19">
-        <f t="shared" ca="1" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="BL16" s="19" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
+      <c r="I16" s="39"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="19"/>
+      <c r="X16" s="19"/>
+      <c r="Y16" s="19"/>
+      <c r="Z16" s="19"/>
+      <c r="AA16" s="19"/>
+      <c r="AB16" s="19"/>
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="19"/>
+      <c r="AE16" s="19"/>
+      <c r="AF16" s="19"/>
+      <c r="AG16" s="19"/>
+      <c r="AH16" s="19"/>
+      <c r="AI16" s="19"/>
+      <c r="AJ16" s="19"/>
+      <c r="AK16" s="19"/>
+      <c r="AL16" s="19"/>
+      <c r="AM16" s="19"/>
+      <c r="AN16" s="19"/>
+      <c r="AO16" s="19"/>
+      <c r="AP16" s="19"/>
+      <c r="AQ16" s="19"/>
+      <c r="AR16" s="19"/>
+      <c r="AS16" s="19"/>
+      <c r="AT16" s="19"/>
+      <c r="AU16" s="19"/>
+      <c r="AV16" s="19"/>
+      <c r="AW16" s="19"/>
+      <c r="AX16" s="19"/>
+      <c r="AY16" s="19"/>
+      <c r="AZ16" s="19"/>
+      <c r="BA16" s="19"/>
+      <c r="BB16" s="19"/>
+      <c r="BC16" s="19"/>
+      <c r="BD16" s="19"/>
+      <c r="BE16" s="19"/>
+      <c r="BF16" s="19"/>
+      <c r="BG16" s="19"/>
+      <c r="BH16" s="19"/>
+      <c r="BI16" s="19"/>
+      <c r="BJ16" s="19"/>
+      <c r="BK16" s="19"/>
+      <c r="BL16" s="19"/>
       <c r="BM16" s="20"/>
     </row>
     <row r="17" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="18" t="s">
-        <v>32</v>
+      <c r="A17" s="4"/>
+      <c r="B17" s="54" t="s">
+        <v>31</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="15">
-        <v>0</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="16">
-        <v>45590</v>
+        <v>45620</v>
       </c>
       <c r="G17" s="17">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H17" s="12"/>
       <c r="I17" s="39" t="str">
@@ -4267,9 +4105,9 @@
         <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
-      <c r="BK17" s="19" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v/>
+      <c r="BK17" s="19">
+        <f t="shared" ca="1" si="7"/>
+        <v>2</v>
       </c>
       <c r="BL17" s="19" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4280,19 +4118,19 @@
     <row r="18" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" s="15">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="F18" s="16">
-        <v>45589</v>
+        <v>45590</v>
       </c>
       <c r="G18" s="17">
         <v>10</v>
@@ -4527,22 +4365,22 @@
     <row r="19" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" s="15">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F19" s="16">
         <v>45589</v>
       </c>
       <c r="G19" s="17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="39" t="str">
@@ -4774,22 +4612,22 @@
     <row r="20" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E20" s="15">
         <v>0</v>
       </c>
       <c r="F20" s="16">
-        <v>45603</v>
+        <v>45589</v>
       </c>
       <c r="G20" s="17">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="39" t="str">
@@ -5018,21 +4856,25 @@
       </c>
       <c r="BM20" s="20"/>
     </row>
-    <row r="21" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="54" t="s">
-        <v>36</v>
+      <c r="B21" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
+        <v>29</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="15">
+        <v>0</v>
+      </c>
       <c r="F21" s="16">
-        <v>45669</v>
+        <v>45603</v>
       </c>
       <c r="G21" s="17">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="39" t="str">
@@ -5263,23 +5105,19 @@
     </row>
     <row r="22" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="18" t="s">
-        <v>37</v>
+      <c r="B22" s="54" t="s">
+        <v>36</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="15">
-        <v>0</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="16">
-        <v>45626</v>
+        <v>45669</v>
       </c>
       <c r="G22" s="17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="39" t="str">
@@ -5511,22 +5349,22 @@
     <row r="23" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E23" s="15">
         <v>0</v>
       </c>
       <c r="F23" s="16">
-        <v>45658</v>
+        <v>45626</v>
       </c>
       <c r="G23" s="17">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="39" t="str">
@@ -5758,13 +5596,13 @@
     <row r="24" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E24" s="15">
         <v>0</v>
@@ -5773,7 +5611,7 @@
         <v>45658</v>
       </c>
       <c r="G24" s="17">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="39" t="str">
@@ -6005,7 +5843,7 @@
     <row r="25" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>26</v>
@@ -6017,10 +5855,10 @@
         <v>0</v>
       </c>
       <c r="F25" s="16">
-        <v>45626</v>
+        <v>45658</v>
       </c>
       <c r="G25" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="39" t="str">
@@ -6148,7 +5986,7 @@
         <v/>
       </c>
       <c r="AN25" s="19" t="str">
-        <f t="shared" ref="AN25" ca="1" si="9">IF(AND($C25="Objetivo",AN$7&gt;=$F25,AN$7&lt;=$F25+$G25-1),2,IF(AND($C25="Marco",AN$7&gt;=$F25,AN$7&lt;=$F25+$G25-1),1,""))</f>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AO25" s="19" t="str">
@@ -6212,7 +6050,7 @@
         <v/>
       </c>
       <c r="BD25" s="19" t="str">
-        <f t="shared" ref="BD25" ca="1" si="10">IF(AND($C25="Objetivo",BD$7&gt;=$F25,BD$7&lt;=$F25+$G25-1),2,IF(AND($C25="Marco",BD$7&gt;=$F25,BD$7&lt;=$F25+$G25-1),1,""))</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
       <c r="BE25" s="19" t="str">
@@ -6248,6 +6086,253 @@
         <v/>
       </c>
       <c r="BM25" s="20"/>
+    </row>
+    <row r="26" spans="1:65" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="15">
+        <v>0</v>
+      </c>
+      <c r="F26" s="16">
+        <v>45626</v>
+      </c>
+      <c r="G26" s="17">
+        <v>30</v>
+      </c>
+      <c r="H26" s="12"/>
+      <c r="I26" s="39" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v/>
+      </c>
+      <c r="J26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="K26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="L26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="M26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="N26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="O26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="P26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="Q26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="R26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="S26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="T26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="U26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="V26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="W26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="X26" s="19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="Y26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="Z26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AA26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AB26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AC26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AD26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AE26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AF26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AG26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AH26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AI26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AJ26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AK26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AL26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AM26" s="19" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="AN26" s="19" t="str">
+        <f t="shared" ref="AN26" ca="1" si="9">IF(AND($C26="Objetivo",AN$7&gt;=$F26,AN$7&lt;=$F26+$G26-1),2,IF(AND($C26="Marco",AN$7&gt;=$F26,AN$7&lt;=$F26+$G26-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="AO26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="AP26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="AQ26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="AR26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="AS26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="AT26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="AU26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="AV26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="AW26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="AX26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="AY26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="AZ26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="BA26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="BB26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="BC26" s="19" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="BD26" s="19" t="str">
+        <f t="shared" ref="BD26" ca="1" si="10">IF(AND($C26="Objetivo",BD$7&gt;=$F26,BD$7&lt;=$F26+$G26-1),2,IF(AND($C26="Marco",BD$7&gt;=$F26,BD$7&lt;=$F26+$G26-1),1,""))</f>
+        <v/>
+      </c>
+      <c r="BE26" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="BF26" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="BG26" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="BH26" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="BI26" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="BJ26" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="BK26" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="BL26" s="19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="BM26" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6260,7 +6345,7 @@
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="S4:V4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:E25">
+  <conditionalFormatting sqref="E9:E26">
     <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6284,12 +6369,12 @@
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL25">
+  <conditionalFormatting sqref="I7:BL26">
     <cfRule type="expression" dxfId="11" priority="7">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10:BL21">
+  <conditionalFormatting sqref="I10:BL22">
     <cfRule type="expression" dxfId="10" priority="194" stopIfTrue="1">
       <formula>AND($C10="Risco Baixo",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
@@ -6306,21 +6391,21 @@
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22:BL25">
+  <conditionalFormatting sqref="I23:BL26">
     <cfRule type="expression" dxfId="5" priority="212" stopIfTrue="1">
-      <formula>AND($C22="Risco Baixo",I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
+      <formula>AND($C23="Risco Baixo",I$7&gt;=$F23,I$7&lt;=$F23+$G23-1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="213" stopIfTrue="1">
-      <formula>AND($C22="Risco Elevado",I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
+      <formula>AND($C23="Risco Elevado",I$7&gt;=$F23,I$7&lt;=$F23+$G23-1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="214" stopIfTrue="1">
-      <formula>AND($C22="Dentro do prazo",I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
+      <formula>AND($C23="Dentro do prazo",I$7&gt;=$F23,I$7&lt;=$F23+$G23-1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="215" stopIfTrue="1">
-      <formula>AND($C22="Risco Médio",I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
+      <formula>AND($C23="Risco Médio",I$7&gt;=$F23,I$7&lt;=$F23+$G23-1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="216" stopIfTrue="1">
-      <formula>AND(LEN($C22)=0,I$7&gt;=$F22,I$7&lt;=$F22+$G22-1)</formula>
+      <formula>AND(LEN($C23)=0,I$7&gt;=$F23,I$7&lt;=$F23+$G23-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
@@ -6332,7 +6417,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C11" xr:uid="{DFFD23FF-9FE8-42D1-8B69-600D9BF05AA3}">
       <formula1>"Objetivo,Marco,Dentro do prazo, Risco Baixo, Risco Médio, Risco Elevado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C25" xr:uid="{A2F07095-4C5B-4F26-9F4F-F9BCE27C6F57}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C26" xr:uid="{A2F07095-4C5B-4F26-9F4F-F9BCE27C6F57}">
       <formula1>"Objetivo,Marco,Dentro do prazo, Risco Baixo, Risco Médio, Risco Elevado"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Incremento de rolagem" prompt="A alteração deste número irá percorrer a vista do Mapa de Gantt." sqref="C7" xr:uid="{40D643B7-C378-45A2-A932-672EA7F96D14}">
@@ -6344,7 +6429,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Um Incremento de Rolagem está na célula C7. _x000a_Meses para as datas na linha 7 são exibidos começando nas células I6 através da célula BL6._x000a_Não modificar estas células. São atualizadas automaticamente com base na data de início do projecto na célula F6." sqref="A6" xr:uid="{C655BEFA-A8F0-47C8-9A9F-B298E206B00E}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Introduzir o Nome da Empresa na célula B4._x000a_Uma lenda está nas células I4 através do AC4. O rótulo da Legenda está na célula G4." sqref="A4" xr:uid="{E8FF6BF3-823C-4A98-BBC9-FA2C64DA9486}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Criar um diagrama de Gantt " sqref="A2" xr:uid="{B30ABCC4-AAAD-48D6-8EEB-7C14721C5981}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D25" xr:uid="{F0D08545-D333-4DCD-8E99-1760350C41F1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D26" xr:uid="{F0D08545-D333-4DCD-8E99-1760350C41F1}">
       <formula1>$C$5:$F$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -6399,7 +6484,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E9:E25</xm:sqref>
+          <xm:sqref>E9:E26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="193" id="{C84307BC-4E4D-4989-9D21-88D6AEB0AFD2}">
@@ -6418,7 +6503,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I10:BL21</xm:sqref>
+          <xm:sqref>I10:BL22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="211" id="{E2F057A2-6D78-42D0-85B8-6A2E32BC0E90}">
@@ -6437,7 +6522,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I22:BL25</xm:sqref>
+          <xm:sqref>I23:BL26</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -6455,25 +6540,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="22a266b9fa9a230c5a512669d8b298c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eddc33fff6b14141ee5c74a0d29ea6a1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6749,6 +6815,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
   <ds:schemaRefs>
@@ -6758,25 +6843,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C87518-DD8E-42CD-8DAC-291A323E849B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6795,4 +6861,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>